<commit_message>
Update word stim list
</commit_message>
<xml_diff>
--- a/stimuli/NAD field.xlsx
+++ b/stimuli/NAD field.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17540" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -522,7 +522,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -679,37 +679,6 @@
       <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -903,7 +872,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -967,10 +936,6 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
@@ -1375,7 +1340,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1383,18 +1348,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q99"/>
+  <dimension ref="A1:P99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:N1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M92" sqref="M92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="16" max="16" width="16.83203125" customWidth="1"/>
+    <col min="15" max="15" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15">
+    <row r="1" spans="1:16" ht="15">
       <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
@@ -1407,104 +1372,95 @@
         <v>1</v>
       </c>
       <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10" t="s">
+      <c r="J1" s="9"/>
+      <c r="K1" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15">
+    <row r="2" spans="1:16" ht="15">
+      <c r="G2" s="8"/>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="10"/>
-    </row>
-    <row r="3" spans="1:17" ht="15">
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" spans="1:16" ht="15">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
       <c r="E3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="F3" s="2"/>
+      <c r="G3" s="13" t="s">
         <v>110</v>
       </c>
+      <c r="H3" s="16"/>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="13" t="s">
+      <c r="K3" s="13" t="s">
         <v>114</v>
       </c>
+      <c r="L3" s="17" t="s">
+        <v>116</v>
+      </c>
       <c r="M3" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="N3" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="O3" s="14"/>
-      <c r="P3" s="17" t="s">
+      <c r="N3" s="14"/>
+      <c r="O3" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="Q3" s="17"/>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="P3" s="17"/>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
       <c r="E4" t="s">
         <v>125</v>
       </c>
+      <c r="G4" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="H4" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="14"/>
+      <c r="K4" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="L4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="J4" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="14"/>
-      <c r="L4" s="18" t="s">
+      <c r="N4" s="14"/>
+      <c r="O4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="N4" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="O4" s="14"/>
-      <c r="P4" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q4" s="19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1514,34 +1470,34 @@
       <c r="E5" t="s">
         <v>20</v>
       </c>
+      <c r="G5" s="20" t="s">
+        <v>20</v>
+      </c>
       <c r="H5" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="14"/>
+      <c r="K5" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="L5" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" s="14"/>
-      <c r="L5" s="20" t="s">
+      <c r="N5" s="14"/>
+      <c r="O5" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="P5" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="M5" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="N5" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="O5" s="14"/>
-      <c r="P5" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q5" s="21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1551,74 +1507,65 @@
       <c r="E6" t="s">
         <v>21</v>
       </c>
+      <c r="G6" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="H6" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="14"/>
+      <c r="K6" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="L6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" s="14"/>
-      <c r="L6" s="22" t="s">
+      <c r="N6" s="14"/>
+      <c r="O6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P6" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="N6" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="O6" s="14"/>
-      <c r="P6" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q6" s="23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
       <c r="E7" t="s">
         <v>22</v>
       </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7">
-        <v>4</v>
-      </c>
+      <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
+      <c r="K7" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="L7" s="63" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="N7" s="63" t="s">
+      <c r="M7" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="O7" s="14"/>
-      <c r="P7" s="17" t="s">
+      <c r="N7" s="14"/>
+      <c r="O7" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="Q7" s="19" t="s">
+      <c r="P7" s="19" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1628,179 +1575,153 @@
       <c r="E8" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
+      <c r="F8" s="62"/>
+      <c r="G8" s="14"/>
       <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14" t="s">
+      <c r="I8" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="K8" s="14"/>
-      <c r="L8" s="20" t="s">
+      <c r="J8" s="14"/>
+      <c r="K8" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="14" t="s">
+      <c r="L8" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="N8" s="20" t="s">
+      <c r="M8" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="14"/>
-      <c r="P8" s="17" t="s">
+      <c r="N8" s="14"/>
+      <c r="O8" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="Q8" s="21" t="s">
+      <c r="P8" s="21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="G9" s="14"/>
       <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14" t="s">
+      <c r="I9" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="K9" s="14"/>
-      <c r="L9" s="22" t="s">
+      <c r="J9" s="14"/>
+      <c r="K9" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="M9" s="14" t="s">
+      <c r="L9" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="N9" s="22" t="s">
+      <c r="M9" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="O9" s="14"/>
-      <c r="P9" s="17" t="s">
+      <c r="N9" s="14"/>
+      <c r="O9" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="Q9" s="23" t="s">
+      <c r="P9" s="23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
       <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G10">
-        <v>4</v>
-      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="14"/>
       <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="15" t="s">
+      <c r="I10" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="K10" s="14"/>
-      <c r="L10" s="18" t="s">
+      <c r="J10" s="14"/>
+      <c r="K10" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="M10" s="15" t="s">
+      <c r="L10" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="N10" s="18" t="s">
+      <c r="M10" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="O10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="17" t="s">
+        <v>36</v>
+      </c>
       <c r="P10" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q10" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>9</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
       </c>
+      <c r="G11" s="14"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="20" t="s">
+      <c r="K11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="L11" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="N11" s="20" t="s">
+      <c r="M11" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="O11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="17" t="s">
+        <v>37</v>
+      </c>
       <c r="P11" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q11" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>126</v>
       </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
       <c r="E12" t="s">
         <v>26</v>
       </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
-      <c r="G12">
-        <v>4</v>
-      </c>
+      <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="22" t="s">
+      <c r="K12" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="M12" s="15" t="s">
+      <c r="L12" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="N12" s="22" t="s">
+      <c r="M12" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="O12" s="14"/>
-      <c r="P12" s="17" t="s">
+      <c r="N12" s="14"/>
+      <c r="O12" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="Q12" s="24" t="s">
+      <c r="P12" s="24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
       <c r="E13" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="G13">
-        <v>4</v>
-      </c>
+      <c r="F13" s="62"/>
+      <c r="G13" s="14"/>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
@@ -1808,33 +1729,22 @@
       <c r="L13" s="14"/>
       <c r="M13" s="14"/>
       <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
+      <c r="O13" s="17" t="s">
+        <v>40</v>
+      </c>
       <c r="P13" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q13" s="17" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
       <c r="E14" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="F14">
-        <v>3</v>
-      </c>
-      <c r="G14">
-        <v>4</v>
-      </c>
+      <c r="F14" s="36"/>
+      <c r="G14" s="14"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
@@ -1842,465 +1752,445 @@
       <c r="L14" s="14"/>
       <c r="M14" s="14"/>
       <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
+      <c r="O14" s="17" t="s">
+        <v>41</v>
+      </c>
       <c r="P14" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q14" s="17" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
+    <row r="15" spans="1:16">
       <c r="E15" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="F15">
-        <v>3</v>
-      </c>
-      <c r="G15">
-        <v>4</v>
-      </c>
+      <c r="F15" s="36"/>
+      <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="17" t="s">
+      <c r="K15" s="17" t="s">
         <v>29</v>
       </c>
+      <c r="L15" s="14"/>
       <c r="M15" s="14"/>
       <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="17" t="s">
+      <c r="O15" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="Q15" s="24" t="s">
+      <c r="P15" s="24" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:16">
       <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="14"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="18" t="s">
+      <c r="K16" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="M16" s="14" t="s">
+      <c r="L16" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="N16" s="18" t="s">
+      <c r="M16" s="18" t="s">
         <v>125</v>
       </c>
+      <c r="N16" s="14"/>
       <c r="O16" s="14"/>
       <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-    </row>
-    <row r="17" spans="6:17">
+    </row>
+    <row r="17" spans="7:16">
+      <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="20" t="s">
+      <c r="K17" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="M17" s="14" t="s">
+      <c r="L17" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="N17" s="20" t="s">
+      <c r="M17" s="20" t="s">
         <v>21</v>
       </c>
+      <c r="N17" s="14"/>
       <c r="O17" s="14"/>
       <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
-    </row>
-    <row r="18" spans="6:17">
+    </row>
+    <row r="18" spans="7:16">
+      <c r="G18" s="14"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="22" t="s">
+      <c r="K18" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="M18" s="14" t="s">
+      <c r="L18" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="N18" s="22" t="s">
+      <c r="M18" s="22" t="s">
         <v>23</v>
       </c>
+      <c r="N18" s="14"/>
       <c r="O18" s="14"/>
       <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-    </row>
-    <row r="19" spans="6:17">
+    </row>
+    <row r="19" spans="7:16">
+      <c r="G19" s="14"/>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="18" t="s">
+      <c r="K19" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="M19" s="14" t="s">
+      <c r="L19" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="N19" s="18" t="s">
+      <c r="M19" s="18" t="s">
         <v>125</v>
       </c>
+      <c r="N19" s="14"/>
       <c r="O19" s="14"/>
       <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-    </row>
-    <row r="20" spans="6:17">
+    </row>
+    <row r="20" spans="7:16">
+      <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="20" t="s">
+      <c r="K20" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="M20" s="14" t="s">
+      <c r="L20" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="N20" s="20" t="s">
+      <c r="M20" s="20" t="s">
         <v>21</v>
       </c>
+      <c r="N20" s="14"/>
       <c r="O20" s="14"/>
       <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-    </row>
-    <row r="21" spans="6:17">
+    </row>
+    <row r="21" spans="7:16">
+      <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="22" t="s">
+      <c r="K21" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="M21" s="14" t="s">
+      <c r="L21" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="N21" s="22" t="s">
+      <c r="M21" s="22" t="s">
         <v>23</v>
       </c>
+      <c r="N21" s="14"/>
       <c r="O21" s="14"/>
       <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-    </row>
-    <row r="22" spans="6:17">
+    </row>
+    <row r="22" spans="7:16">
+      <c r="G22" s="14"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="18" t="s">
+      <c r="K22" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="M22" s="15" t="s">
+      <c r="L22" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="N22" s="18" t="s">
+      <c r="M22" s="18" t="s">
         <v>125</v>
       </c>
+      <c r="N22" s="14"/>
       <c r="O22" s="14"/>
       <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
-    </row>
-    <row r="23" spans="6:17">
+    </row>
+    <row r="23" spans="7:16">
+      <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="20" t="s">
+      <c r="K23" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="M23" s="15" t="s">
+      <c r="L23" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="N23" s="20" t="s">
+      <c r="M23" s="20" t="s">
         <v>21</v>
       </c>
+      <c r="N23" s="14"/>
       <c r="O23" s="14"/>
       <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
-    </row>
-    <row r="24" spans="6:17">
+    </row>
+    <row r="24" spans="7:16">
+      <c r="G24" s="14"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="22" t="s">
+      <c r="K24" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="M24" s="15" t="s">
+      <c r="L24" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="N24" s="22" t="s">
+      <c r="M24" s="22" t="s">
         <v>23</v>
       </c>
+      <c r="N24" s="14"/>
       <c r="O24" s="14"/>
       <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
-    </row>
-    <row r="27" spans="6:17">
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="6:17" ht="15">
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="25" t="s">
+    </row>
+    <row r="28" spans="7:16" ht="15">
+      <c r="G28" s="25" t="s">
         <v>113</v>
       </c>
+      <c r="H28" s="26"/>
       <c r="I28" s="26"/>
       <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="25" t="s">
+      <c r="K28" s="25" t="s">
         <v>114</v>
       </c>
+      <c r="L28" s="28" t="s">
+        <v>116</v>
+      </c>
       <c r="M28" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="N28" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="O28" s="27"/>
-      <c r="P28" s="28" t="s">
+      <c r="N28" s="27"/>
+      <c r="O28" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="Q28" s="28"/>
-    </row>
-    <row r="29" spans="6:17">
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
+      <c r="P28" s="28"/>
+    </row>
+    <row r="29" spans="7:16">
+      <c r="G29" s="29" t="s">
+        <v>23</v>
+      </c>
       <c r="H29" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="J29" s="27"/>
+      <c r="K29" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="I29" s="29" t="s">
+      <c r="L29" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="M29" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="30" t="s">
+      <c r="N29" s="27"/>
+      <c r="O29" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="P29" s="31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="7:16">
+      <c r="G30" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="I30" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="J30" s="27"/>
+      <c r="K30" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="L30" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="K29" s="27"/>
-      <c r="L29" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="M29" s="30" t="s">
+      <c r="M30" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="N30" s="27"/>
+      <c r="O30" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="P30" s="33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="7:16">
+      <c r="G31" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="H31" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="I31" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="J31" s="27"/>
+      <c r="K31" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="L31" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="N29" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="O29" s="27"/>
-      <c r="P29" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q29" s="31" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="6:17">
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="I30" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="J30" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="K30" s="27"/>
-      <c r="L30" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="M30" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="N30" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="O30" s="27"/>
-      <c r="P30" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q30" s="33" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="6:17">
-      <c r="H31" s="34" t="s">
+      <c r="M31" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="N31" s="27"/>
+      <c r="O31" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="P31" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="I31" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="J31" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="K31" s="27"/>
-      <c r="L31" s="34" t="s">
-        <v>128</v>
-      </c>
-      <c r="M31" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="N31" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="O31" s="27"/>
-      <c r="P31" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q31" s="35" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="32" spans="6:17">
+    </row>
+    <row r="32" spans="7:16">
+      <c r="G32" s="27"/>
       <c r="H32" s="27"/>
       <c r="I32" s="27"/>
       <c r="J32" s="27"/>
-      <c r="K32" s="27"/>
-      <c r="L32" s="29" t="s">
+      <c r="K32" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="M32" s="27" t="s">
+      <c r="L32" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="N32" s="29" t="s">
+      <c r="M32" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="O32" s="27"/>
-      <c r="P32" s="28" t="s">
+      <c r="N32" s="27"/>
+      <c r="O32" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="Q32" s="31" t="s">
+      <c r="P32" s="31" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="8:17">
+    <row r="33" spans="7:16">
+      <c r="G33" s="27"/>
       <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27" t="s">
+      <c r="I33" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="K33" s="27"/>
-      <c r="L33" s="32" t="s">
+      <c r="J33" s="27"/>
+      <c r="K33" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="M33" s="27" t="s">
+      <c r="L33" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="N33" s="32" t="s">
+      <c r="M33" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="O33" s="27"/>
-      <c r="P33" s="28" t="s">
+      <c r="N33" s="27"/>
+      <c r="O33" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="Q33" s="33" t="s">
+      <c r="P33" s="33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="8:17">
+    <row r="34" spans="7:16">
+      <c r="G34" s="27"/>
       <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
-      <c r="J34" s="27" t="s">
+      <c r="I34" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="K34" s="27"/>
-      <c r="L34" s="34" t="s">
+      <c r="J34" s="27"/>
+      <c r="K34" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="M34" s="27" t="s">
+      <c r="L34" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="N34" s="34" t="s">
+      <c r="M34" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="O34" s="27"/>
-      <c r="P34" s="28" t="s">
+      <c r="N34" s="27"/>
+      <c r="O34" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="Q34" s="35" t="s">
+      <c r="P34" s="35" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="8:17">
+    <row r="35" spans="7:16">
+      <c r="G35" s="27"/>
       <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="27" t="s">
+      <c r="I35" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="K35" s="27"/>
-      <c r="L35" s="29" t="s">
+      <c r="J35" s="27"/>
+      <c r="K35" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="M35" s="27" t="s">
+      <c r="L35" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="N35" s="29" t="s">
+      <c r="M35" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="O35" s="27"/>
+      <c r="N35" s="27"/>
+      <c r="O35" s="28" t="s">
+        <v>36</v>
+      </c>
       <c r="P35" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q35" s="28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="8:17">
+    <row r="36" spans="7:16">
+      <c r="G36" s="27"/>
       <c r="H36" s="27"/>
       <c r="I36" s="27"/>
       <c r="J36" s="27"/>
-      <c r="K36" s="27"/>
-      <c r="L36" s="32" t="s">
+      <c r="K36" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="M36" s="27" t="s">
+      <c r="L36" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="N36" s="32" t="s">
+      <c r="M36" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="O36" s="27"/>
+      <c r="N36" s="27"/>
+      <c r="O36" s="28" t="s">
+        <v>37</v>
+      </c>
       <c r="P36" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q36" s="28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="8:17">
+    <row r="37" spans="7:16">
+      <c r="G37" s="27"/>
       <c r="H37" s="27"/>
       <c r="I37" s="27"/>
       <c r="J37" s="27"/>
-      <c r="K37" s="27"/>
-      <c r="L37" s="34" t="s">
+      <c r="K37" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="M37" s="27" t="s">
+      <c r="L37" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="N37" s="34" t="s">
+      <c r="M37" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="O37" s="27"/>
+      <c r="N37" s="27"/>
+      <c r="O37" s="28" t="s">
+        <v>38</v>
+      </c>
       <c r="P37" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q37" s="28" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="38" spans="8:17">
+    <row r="38" spans="7:16">
+      <c r="G38" s="27"/>
       <c r="H38" s="27"/>
       <c r="I38" s="27"/>
       <c r="J38" s="27"/>
@@ -2308,15 +2198,15 @@
       <c r="L38" s="27"/>
       <c r="M38" s="27"/>
       <c r="N38" s="27"/>
-      <c r="O38" s="27"/>
+      <c r="O38" s="28" t="s">
+        <v>40</v>
+      </c>
       <c r="P38" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q38" s="28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="8:17">
+    <row r="39" spans="7:16">
+      <c r="G39" s="27"/>
       <c r="H39" s="27"/>
       <c r="I39" s="27"/>
       <c r="J39" s="27"/>
@@ -2324,1117 +2214,1116 @@
       <c r="L39" s="27"/>
       <c r="M39" s="27"/>
       <c r="N39" s="27"/>
-      <c r="O39" s="27"/>
+      <c r="O39" s="28" t="s">
+        <v>41</v>
+      </c>
       <c r="P39" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q39" s="28" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="40" spans="8:17">
+    <row r="40" spans="7:16">
+      <c r="G40" s="27"/>
       <c r="H40" s="27"/>
       <c r="I40" s="27"/>
       <c r="J40" s="27"/>
-      <c r="K40" s="27"/>
-      <c r="L40" s="28" t="s">
+      <c r="K40" s="28" t="s">
         <v>29</v>
       </c>
+      <c r="L40" s="27"/>
       <c r="M40" s="27"/>
       <c r="N40" s="27"/>
-      <c r="O40" s="27"/>
+      <c r="O40" s="28" t="s">
+        <v>42</v>
+      </c>
       <c r="P40" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q40" s="28" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="41" spans="8:17">
+    <row r="41" spans="7:16">
+      <c r="G41" s="27"/>
       <c r="H41" s="27"/>
       <c r="I41" s="27"/>
       <c r="J41" s="27"/>
-      <c r="K41" s="27"/>
-      <c r="L41" s="29" t="s">
+      <c r="K41" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="M41" s="27" t="s">
+      <c r="L41" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="N41" s="29" t="s">
+      <c r="M41" s="29" t="s">
         <v>20</v>
       </c>
+      <c r="N41" s="27"/>
       <c r="O41" s="27"/>
       <c r="P41" s="27"/>
-      <c r="Q41" s="27"/>
-    </row>
-    <row r="42" spans="8:17">
+    </row>
+    <row r="42" spans="7:16">
+      <c r="G42" s="27"/>
       <c r="H42" s="27"/>
       <c r="I42" s="27"/>
       <c r="J42" s="27"/>
-      <c r="K42" s="27"/>
-      <c r="L42" s="32" t="s">
+      <c r="K42" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="M42" s="27" t="s">
+      <c r="L42" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="N42" s="32" t="s">
+      <c r="M42" s="32" t="s">
         <v>25</v>
       </c>
+      <c r="N42" s="27"/>
       <c r="O42" s="27"/>
       <c r="P42" s="27"/>
-      <c r="Q42" s="27"/>
-    </row>
-    <row r="43" spans="8:17">
+    </row>
+    <row r="43" spans="7:16">
+      <c r="G43" s="27"/>
       <c r="H43" s="27"/>
       <c r="I43" s="27"/>
       <c r="J43" s="27"/>
-      <c r="K43" s="27"/>
-      <c r="L43" s="34" t="s">
+      <c r="K43" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="M43" s="27" t="s">
+      <c r="L43" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="N43" s="34" t="s">
+      <c r="M43" s="34" t="s">
         <v>24</v>
       </c>
+      <c r="N43" s="27"/>
       <c r="O43" s="27"/>
       <c r="P43" s="27"/>
-      <c r="Q43" s="27"/>
-    </row>
-    <row r="44" spans="8:17">
+    </row>
+    <row r="44" spans="7:16">
+      <c r="G44" s="27"/>
       <c r="H44" s="27"/>
       <c r="I44" s="27"/>
       <c r="J44" s="27"/>
-      <c r="K44" s="27"/>
-      <c r="L44" s="29" t="s">
+      <c r="K44" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="M44" s="27" t="s">
+      <c r="L44" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="N44" s="29" t="s">
+      <c r="M44" s="29" t="s">
         <v>20</v>
       </c>
+      <c r="N44" s="27"/>
       <c r="O44" s="27"/>
       <c r="P44" s="27"/>
-      <c r="Q44" s="27"/>
-    </row>
-    <row r="45" spans="8:17">
+    </row>
+    <row r="45" spans="7:16">
+      <c r="G45" s="27"/>
       <c r="H45" s="27"/>
       <c r="I45" s="27"/>
       <c r="J45" s="27"/>
-      <c r="K45" s="27"/>
-      <c r="L45" s="32" t="s">
+      <c r="K45" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="M45" s="27" t="s">
+      <c r="L45" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="N45" s="32" t="s">
+      <c r="M45" s="32" t="s">
         <v>25</v>
       </c>
+      <c r="N45" s="27"/>
       <c r="O45" s="27"/>
       <c r="P45" s="27"/>
-      <c r="Q45" s="27"/>
-    </row>
-    <row r="46" spans="8:17">
+    </row>
+    <row r="46" spans="7:16">
+      <c r="G46" s="27"/>
       <c r="H46" s="27"/>
       <c r="I46" s="27"/>
       <c r="J46" s="27"/>
-      <c r="K46" s="27"/>
-      <c r="L46" s="34" t="s">
+      <c r="K46" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="M46" s="27" t="s">
+      <c r="L46" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="N46" s="34" t="s">
+      <c r="M46" s="34" t="s">
         <v>24</v>
       </c>
+      <c r="N46" s="27"/>
       <c r="O46" s="27"/>
       <c r="P46" s="27"/>
-      <c r="Q46" s="27"/>
-    </row>
-    <row r="47" spans="8:17">
+    </row>
+    <row r="47" spans="7:16">
+      <c r="G47" s="27"/>
       <c r="H47" s="27"/>
       <c r="I47" s="27"/>
       <c r="J47" s="27"/>
-      <c r="K47" s="27"/>
-      <c r="L47" s="29" t="s">
+      <c r="K47" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="M47" s="27" t="s">
+      <c r="L47" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="N47" s="29" t="s">
+      <c r="M47" s="29" t="s">
         <v>20</v>
       </c>
+      <c r="N47" s="27"/>
       <c r="O47" s="27"/>
       <c r="P47" s="27"/>
-      <c r="Q47" s="27"/>
-    </row>
-    <row r="48" spans="8:17">
+    </row>
+    <row r="48" spans="7:16">
+      <c r="G48" s="27"/>
       <c r="H48" s="27"/>
       <c r="I48" s="27"/>
       <c r="J48" s="27"/>
-      <c r="K48" s="27"/>
-      <c r="L48" s="32" t="s">
+      <c r="K48" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="M48" s="27" t="s">
+      <c r="L48" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="N48" s="32" t="s">
+      <c r="M48" s="32" t="s">
         <v>25</v>
       </c>
+      <c r="N48" s="27"/>
       <c r="O48" s="27"/>
       <c r="P48" s="27"/>
-      <c r="Q48" s="27"/>
-    </row>
-    <row r="49" spans="8:17">
+    </row>
+    <row r="49" spans="7:16">
+      <c r="G49" s="27"/>
       <c r="H49" s="27"/>
       <c r="I49" s="27"/>
       <c r="J49" s="27"/>
-      <c r="K49" s="27"/>
-      <c r="L49" s="34" t="s">
+      <c r="K49" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="M49" s="27" t="s">
+      <c r="L49" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="N49" s="34" t="s">
+      <c r="M49" s="34" t="s">
         <v>24</v>
       </c>
+      <c r="N49" s="27"/>
       <c r="O49" s="27"/>
       <c r="P49" s="27"/>
-      <c r="Q49" s="27"/>
-    </row>
-    <row r="50" spans="8:17" s="36" customFormat="1">
-      <c r="L50" s="61"/>
-      <c r="N50" s="61"/>
-    </row>
-    <row r="51" spans="8:17" s="36" customFormat="1">
-      <c r="L51" s="61"/>
-      <c r="N51" s="61"/>
-    </row>
-    <row r="52" spans="8:17" s="36" customFormat="1">
-      <c r="L52" s="61"/>
-      <c r="N52" s="61"/>
-    </row>
-    <row r="53" spans="8:17" ht="15">
-      <c r="H53" s="37" t="s">
+    </row>
+    <row r="50" spans="7:16" s="36" customFormat="1">
+      <c r="K50" s="61"/>
+      <c r="M50" s="61"/>
+    </row>
+    <row r="51" spans="7:16" s="36" customFormat="1">
+      <c r="K51" s="61"/>
+      <c r="M51" s="61"/>
+    </row>
+    <row r="52" spans="7:16" s="36" customFormat="1">
+      <c r="K52" s="61"/>
+      <c r="M52" s="61"/>
+    </row>
+    <row r="53" spans="7:16" ht="15">
+      <c r="G53" s="37" t="s">
         <v>117</v>
       </c>
+      <c r="H53" s="37"/>
       <c r="I53" s="37"/>
       <c r="J53" s="37"/>
-      <c r="K53" s="37"/>
-      <c r="L53" s="37" t="s">
+      <c r="K53" s="37" t="s">
         <v>114</v>
       </c>
+      <c r="L53" s="39" t="s">
+        <v>116</v>
+      </c>
       <c r="M53" s="39" t="s">
-        <v>116</v>
-      </c>
-      <c r="N53" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="O53" s="38"/>
-      <c r="P53" s="39" t="s">
+      <c r="N53" s="38"/>
+      <c r="O53" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="Q53" s="39"/>
-    </row>
-    <row r="54" spans="8:17">
+      <c r="P53" s="39"/>
+    </row>
+    <row r="54" spans="7:16">
+      <c r="G54" s="40" t="s">
+        <v>125</v>
+      </c>
       <c r="H54" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="I54" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="J54" s="38"/>
+      <c r="K54" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="I54" s="40" t="s">
+      <c r="L54" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="M54" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="J54" s="41" t="s">
+      <c r="N54" s="38"/>
+      <c r="O54" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="P54" s="42" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="7:16">
+      <c r="G55" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="H55" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="I55" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="J55" s="38"/>
+      <c r="K55" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="L55" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="K54" s="38"/>
-      <c r="L54" s="40" t="s">
+      <c r="M55" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="N55" s="38"/>
+      <c r="O55" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="P55" s="44" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="7:16">
+      <c r="G56" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="H56" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="I56" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="J56" s="38"/>
+      <c r="K56" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="L56" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="M56" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="N56" s="38"/>
+      <c r="O56" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="P56" s="46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="7:16">
+      <c r="G57" s="38"/>
+      <c r="H57" s="38"/>
+      <c r="I57" s="41"/>
+      <c r="J57" s="38"/>
+      <c r="K57" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="M54" s="41" t="s">
+      <c r="L57" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="M57" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="N57" s="38"/>
+      <c r="O57" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="P57" s="42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="58" spans="7:16">
+      <c r="G58" s="38"/>
+      <c r="H58" s="38"/>
+      <c r="I58" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="J58" s="38"/>
+      <c r="K58" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="L58" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="M58" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="N58" s="38"/>
+      <c r="O58" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="P58" s="44" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="59" spans="7:16">
+      <c r="G59" s="38"/>
+      <c r="H59" s="38"/>
+      <c r="I59" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="J59" s="38"/>
+      <c r="K59" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="L59" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="M59" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="N59" s="38"/>
+      <c r="O59" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="P59" s="46" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="7:16">
+      <c r="G60" s="38"/>
+      <c r="H60" s="38"/>
+      <c r="I60" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="J60" s="38"/>
+      <c r="K60" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="L60" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="M60" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="N60" s="38"/>
+      <c r="O60" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="P60" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="N54" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="O54" s="38"/>
-      <c r="P54" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q54" s="42" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="55" spans="8:17">
-      <c r="H55" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="I55" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="J55" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="K55" s="38"/>
-      <c r="L55" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="M55" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="N55" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="O55" s="38"/>
-      <c r="P55" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q55" s="44" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="56" spans="8:17">
-      <c r="H56" s="45" t="s">
-        <v>20</v>
-      </c>
-      <c r="I56" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="J56" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="K56" s="38"/>
-      <c r="L56" s="45" t="s">
-        <v>20</v>
-      </c>
-      <c r="M56" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="N56" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="O56" s="38"/>
-      <c r="P56" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q56" s="46" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="57" spans="8:17">
-      <c r="H57" s="38"/>
-      <c r="I57" s="38"/>
-      <c r="J57" s="41"/>
-      <c r="K57" s="38"/>
-      <c r="L57" s="40" t="s">
-        <v>125</v>
-      </c>
-      <c r="M57" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="N57" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="O57" s="38"/>
-      <c r="P57" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q57" s="42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="58" spans="8:17">
-      <c r="H58" s="38"/>
-      <c r="I58" s="38"/>
-      <c r="J58" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="K58" s="38"/>
-      <c r="L58" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="M58" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="N58" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="O58" s="38"/>
-      <c r="P58" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q58" s="44" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="59" spans="8:17">
-      <c r="H59" s="38"/>
-      <c r="I59" s="38"/>
-      <c r="J59" s="41" t="s">
-        <v>127</v>
-      </c>
-      <c r="K59" s="38"/>
-      <c r="L59" s="45" t="s">
-        <v>20</v>
-      </c>
-      <c r="M59" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="N59" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="O59" s="38"/>
-      <c r="P59" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q59" s="46" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="60" spans="8:17">
-      <c r="H60" s="38"/>
-      <c r="I60" s="38"/>
-      <c r="J60" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="K60" s="38"/>
-      <c r="L60" s="40" t="s">
-        <v>125</v>
-      </c>
-      <c r="M60" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="N60" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="O60" s="38"/>
-      <c r="P60" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q60" s="47" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="61" spans="8:17">
+    </row>
+    <row r="61" spans="7:16">
+      <c r="G61" s="38"/>
       <c r="H61" s="38"/>
       <c r="I61" s="38"/>
       <c r="J61" s="38"/>
-      <c r="K61" s="38"/>
-      <c r="L61" s="43" t="s">
+      <c r="K61" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="M61" s="41" t="s">
+      <c r="L61" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="N61" s="43" t="s">
+      <c r="M61" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="O61" s="38"/>
-      <c r="P61" s="39" t="s">
+      <c r="N61" s="38"/>
+      <c r="O61" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="Q61" s="47" t="s">
+      <c r="P61" s="47" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="8:17">
+    <row r="62" spans="7:16">
+      <c r="G62" s="38"/>
       <c r="H62" s="38"/>
       <c r="I62" s="38"/>
       <c r="J62" s="38"/>
-      <c r="K62" s="38"/>
-      <c r="L62" s="45" t="s">
+      <c r="K62" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="M62" s="41" t="s">
+      <c r="L62" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="N62" s="45" t="s">
+      <c r="M62" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="O62" s="38"/>
-      <c r="P62" s="39" t="s">
+      <c r="N62" s="38"/>
+      <c r="O62" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="Q62" s="47" t="s">
+      <c r="P62" s="47" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="8:17">
+    <row r="63" spans="7:16">
+      <c r="G63" s="38"/>
       <c r="H63" s="38"/>
       <c r="I63" s="38"/>
       <c r="J63" s="38"/>
-      <c r="K63" s="38"/>
-      <c r="L63" s="45"/>
-      <c r="M63" s="41"/>
-      <c r="N63" s="45"/>
-      <c r="O63" s="38"/>
+      <c r="K63" s="45"/>
+      <c r="L63" s="41"/>
+      <c r="M63" s="45"/>
+      <c r="N63" s="38"/>
+      <c r="O63" s="39" t="s">
+        <v>40</v>
+      </c>
       <c r="P63" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q63" s="39" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="64" spans="8:17">
+    <row r="64" spans="7:16">
+      <c r="G64" s="38"/>
       <c r="H64" s="38"/>
       <c r="I64" s="38"/>
       <c r="J64" s="38"/>
-      <c r="K64" s="38"/>
-      <c r="L64" s="45"/>
-      <c r="M64" s="41"/>
-      <c r="N64" s="45"/>
-      <c r="O64" s="38"/>
+      <c r="K64" s="45"/>
+      <c r="L64" s="41"/>
+      <c r="M64" s="45"/>
+      <c r="N64" s="38"/>
+      <c r="O64" s="39" t="s">
+        <v>41</v>
+      </c>
       <c r="P64" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q64" s="39" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="8:17">
+    <row r="65" spans="7:16">
+      <c r="G65" s="38"/>
       <c r="H65" s="38"/>
       <c r="I65" s="38"/>
       <c r="J65" s="38"/>
-      <c r="K65" s="38"/>
-      <c r="L65" s="39" t="s">
+      <c r="K65" s="39" t="s">
         <v>29</v>
       </c>
+      <c r="L65" s="38"/>
       <c r="M65" s="38"/>
       <c r="N65" s="38"/>
-      <c r="O65" s="38"/>
+      <c r="O65" s="39" t="s">
+        <v>42</v>
+      </c>
       <c r="P65" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q65" s="39" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="66" spans="8:17">
+    <row r="66" spans="7:16">
+      <c r="G66" s="38"/>
       <c r="H66" s="38"/>
       <c r="I66" s="38"/>
       <c r="J66" s="38"/>
-      <c r="K66" s="38"/>
-      <c r="L66" s="40" t="s">
+      <c r="K66" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="M66" s="41" t="s">
+      <c r="L66" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="N66" s="40" t="s">
+      <c r="M66" s="40" t="s">
         <v>21</v>
       </c>
+      <c r="N66" s="38"/>
       <c r="O66" s="38"/>
       <c r="P66" s="38"/>
-      <c r="Q66" s="38"/>
-    </row>
-    <row r="67" spans="8:17">
+    </row>
+    <row r="67" spans="7:16">
+      <c r="G67" s="38"/>
       <c r="H67" s="38"/>
       <c r="I67" s="38"/>
       <c r="J67" s="38"/>
-      <c r="K67" s="38"/>
-      <c r="L67" s="43" t="s">
+      <c r="K67" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="M67" s="41" t="s">
+      <c r="L67" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="N67" s="43" t="s">
+      <c r="M67" s="43" t="s">
         <v>128</v>
       </c>
+      <c r="N67" s="38"/>
       <c r="O67" s="38"/>
       <c r="P67" s="38"/>
-      <c r="Q67" s="38"/>
-    </row>
-    <row r="68" spans="8:17">
+    </row>
+    <row r="68" spans="7:16">
+      <c r="G68" s="38"/>
       <c r="H68" s="38"/>
       <c r="I68" s="38"/>
       <c r="J68" s="38"/>
-      <c r="K68" s="38"/>
-      <c r="L68" s="45" t="s">
+      <c r="K68" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="M68" s="41" t="s">
+      <c r="L68" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="N68" s="45" t="s">
+      <c r="M68" s="45" t="s">
         <v>24</v>
       </c>
+      <c r="N68" s="38"/>
       <c r="O68" s="38"/>
       <c r="P68" s="38"/>
-      <c r="Q68" s="38"/>
-    </row>
-    <row r="69" spans="8:17">
+    </row>
+    <row r="69" spans="7:16">
+      <c r="G69" s="38"/>
       <c r="H69" s="38"/>
       <c r="I69" s="38"/>
       <c r="J69" s="38"/>
-      <c r="K69" s="38"/>
-      <c r="L69" s="40" t="s">
+      <c r="K69" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="M69" s="41" t="s">
+      <c r="L69" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="N69" s="40" t="s">
+      <c r="M69" s="40" t="s">
         <v>21</v>
       </c>
+      <c r="N69" s="38"/>
       <c r="O69" s="38"/>
       <c r="P69" s="38"/>
-      <c r="Q69" s="38"/>
-    </row>
-    <row r="70" spans="8:17">
+    </row>
+    <row r="70" spans="7:16">
+      <c r="G70" s="38"/>
       <c r="H70" s="38"/>
       <c r="I70" s="38"/>
       <c r="J70" s="38"/>
-      <c r="K70" s="38"/>
-      <c r="L70" s="43" t="s">
+      <c r="K70" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="M70" s="41" t="s">
+      <c r="L70" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="N70" s="43" t="s">
+      <c r="M70" s="43" t="s">
         <v>128</v>
       </c>
+      <c r="N70" s="38"/>
       <c r="O70" s="38"/>
       <c r="P70" s="38"/>
-      <c r="Q70" s="38"/>
-    </row>
-    <row r="71" spans="8:17">
+    </row>
+    <row r="71" spans="7:16">
+      <c r="G71" s="38"/>
       <c r="H71" s="38"/>
       <c r="I71" s="38"/>
       <c r="J71" s="38"/>
-      <c r="K71" s="38"/>
-      <c r="L71" s="45" t="s">
+      <c r="K71" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="M71" s="41" t="s">
+      <c r="L71" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="N71" s="45" t="s">
+      <c r="M71" s="45" t="s">
         <v>24</v>
       </c>
+      <c r="N71" s="38"/>
       <c r="O71" s="38"/>
       <c r="P71" s="38"/>
-      <c r="Q71" s="38"/>
-    </row>
-    <row r="72" spans="8:17">
+    </row>
+    <row r="72" spans="7:16">
+      <c r="G72" s="38"/>
       <c r="H72" s="38"/>
       <c r="I72" s="38"/>
       <c r="J72" s="38"/>
-      <c r="K72" s="38"/>
-      <c r="L72" s="40" t="s">
+      <c r="K72" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="M72" s="41" t="s">
+      <c r="L72" s="41" t="s">
         <v>129</v>
       </c>
-      <c r="N72" s="40" t="s">
+      <c r="M72" s="40" t="s">
         <v>21</v>
       </c>
+      <c r="N72" s="38"/>
       <c r="O72" s="38"/>
       <c r="P72" s="38"/>
-      <c r="Q72" s="38"/>
-    </row>
-    <row r="73" spans="8:17">
+    </row>
+    <row r="73" spans="7:16">
+      <c r="G73" s="38"/>
       <c r="H73" s="38"/>
       <c r="I73" s="38"/>
       <c r="J73" s="38"/>
-      <c r="K73" s="38"/>
-      <c r="L73" s="43" t="s">
+      <c r="K73" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="M73" s="41" t="s">
+      <c r="L73" s="41" t="s">
         <v>129</v>
       </c>
-      <c r="N73" s="43" t="s">
+      <c r="M73" s="43" t="s">
         <v>128</v>
       </c>
+      <c r="N73" s="38"/>
       <c r="O73" s="38"/>
       <c r="P73" s="38"/>
-      <c r="Q73" s="38"/>
-    </row>
-    <row r="74" spans="8:17">
+    </row>
+    <row r="74" spans="7:16">
+      <c r="G74" s="38"/>
       <c r="H74" s="38"/>
       <c r="I74" s="38"/>
       <c r="J74" s="38"/>
-      <c r="K74" s="38"/>
-      <c r="L74" s="45" t="s">
+      <c r="K74" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="M74" s="41" t="s">
+      <c r="L74" s="41" t="s">
         <v>129</v>
       </c>
-      <c r="N74" s="45" t="s">
+      <c r="M74" s="45" t="s">
         <v>24</v>
       </c>
+      <c r="N74" s="38"/>
       <c r="O74" s="38"/>
       <c r="P74" s="38"/>
-      <c r="Q74" s="38"/>
-    </row>
-    <row r="78" spans="8:17" ht="18">
-      <c r="H78" s="48" t="s">
+    </row>
+    <row r="78" spans="7:16" ht="18">
+      <c r="G78" s="48" t="s">
         <v>119</v>
       </c>
+      <c r="H78" s="49"/>
       <c r="I78" s="49"/>
-      <c r="J78" s="49"/>
-      <c r="K78" s="60"/>
+      <c r="J78" s="60"/>
+      <c r="K78" s="60" t="s">
+        <v>114</v>
+      </c>
       <c r="L78" s="60" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="M78" s="60" t="s">
-        <v>116</v>
-      </c>
-      <c r="N78" s="60" t="s">
         <v>115</v>
       </c>
-      <c r="O78" s="50"/>
-      <c r="P78" s="51" t="s">
+      <c r="N78" s="50"/>
+      <c r="O78" s="51" t="s">
         <v>118</v>
       </c>
-      <c r="Q78" s="51"/>
-    </row>
-    <row r="79" spans="8:17">
+      <c r="P78" s="51"/>
+    </row>
+    <row r="79" spans="7:16">
+      <c r="G79" s="52" t="s">
+        <v>22</v>
+      </c>
       <c r="H79" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="I79" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="J79" s="50"/>
+      <c r="K79" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="I79" s="52" t="s">
+      <c r="L79" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="M79" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="J79" s="53" t="s">
+      <c r="N79" s="50"/>
+      <c r="O79" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="P79" s="54" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="80" spans="7:16">
+      <c r="G80" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="H80" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="I80" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="J80" s="50"/>
+      <c r="K80" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="L80" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="K79" s="50"/>
-      <c r="L79" s="52" t="s">
-        <v>22</v>
-      </c>
-      <c r="M79" s="53" t="s">
+      <c r="M80" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="N80" s="50"/>
+      <c r="O80" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="P80" s="56" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" spans="7:16">
+      <c r="G81" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="H81" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="I81" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="J81" s="50"/>
+      <c r="K81" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="L81" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="N79" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="O79" s="50"/>
-      <c r="P79" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q79" s="54" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="80" spans="8:17">
-      <c r="H80" s="55" t="s">
-        <v>27</v>
-      </c>
-      <c r="I80" s="55" t="s">
-        <v>125</v>
-      </c>
-      <c r="J80" s="53" t="s">
-        <v>128</v>
-      </c>
-      <c r="K80" s="50"/>
-      <c r="L80" s="55" t="s">
-        <v>27</v>
-      </c>
-      <c r="M80" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="N80" s="55" t="s">
-        <v>125</v>
-      </c>
-      <c r="O80" s="50"/>
-      <c r="P80" s="51" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q80" s="56" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="81" spans="8:17">
-      <c r="H81" s="57" t="s">
+      <c r="M81" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="N81" s="50"/>
+      <c r="O81" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="P81" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="I81" s="57" t="s">
-        <v>20</v>
-      </c>
-      <c r="J81" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="K81" s="50"/>
-      <c r="L81" s="57" t="s">
-        <v>21</v>
-      </c>
-      <c r="M81" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="N81" s="57" t="s">
-        <v>20</v>
-      </c>
-      <c r="O81" s="50"/>
-      <c r="P81" s="51" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q81" s="58" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="82" spans="8:17">
+    </row>
+    <row r="82" spans="7:16">
+      <c r="G82" s="50"/>
       <c r="H82" s="50"/>
       <c r="I82" s="50"/>
       <c r="J82" s="50"/>
-      <c r="K82" s="50"/>
-      <c r="L82" s="52" t="s">
+      <c r="K82" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="M82" s="53" t="s">
+      <c r="L82" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="N82" s="52" t="s">
+      <c r="M82" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="O82" s="50"/>
-      <c r="P82" s="51" t="s">
+      <c r="N82" s="50"/>
+      <c r="O82" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="Q82" s="54" t="s">
+      <c r="P82" s="54" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="8:17">
+    <row r="83" spans="7:16">
+      <c r="G83" s="50"/>
       <c r="H83" s="50"/>
-      <c r="I83" s="50"/>
-      <c r="J83" s="59" t="s">
+      <c r="I83" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="K83" s="50"/>
-      <c r="L83" s="55" t="s">
+      <c r="J83" s="50"/>
+      <c r="K83" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="M83" s="53" t="s">
+      <c r="L83" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="N83" s="55" t="s">
+      <c r="M83" s="55" t="s">
         <v>125</v>
       </c>
-      <c r="O83" s="50"/>
-      <c r="P83" s="51" t="s">
+      <c r="N83" s="50"/>
+      <c r="O83" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="Q83" s="56" t="s">
+      <c r="P83" s="56" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="84" spans="8:17">
+    <row r="84" spans="7:16">
+      <c r="G84" s="50"/>
       <c r="H84" s="50"/>
-      <c r="I84" s="50"/>
-      <c r="J84" s="59" t="s">
+      <c r="I84" s="59" t="s">
         <v>127</v>
       </c>
-      <c r="K84" s="50"/>
-      <c r="L84" s="57" t="s">
+      <c r="J84" s="50"/>
+      <c r="K84" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="M84" s="53" t="s">
+      <c r="L84" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="N84" s="57" t="s">
+      <c r="M84" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="O84" s="50"/>
-      <c r="P84" s="51" t="s">
+      <c r="N84" s="50"/>
+      <c r="O84" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="Q84" s="58" t="s">
+      <c r="P84" s="58" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="8:17">
+    <row r="85" spans="7:16">
+      <c r="G85" s="50"/>
       <c r="H85" s="50"/>
-      <c r="I85" s="50"/>
-      <c r="J85" s="59" t="s">
+      <c r="I85" s="59" t="s">
         <v>129</v>
       </c>
-      <c r="K85" s="50"/>
-      <c r="L85" s="52" t="s">
+      <c r="J85" s="50"/>
+      <c r="K85" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="M85" s="53" t="s">
+      <c r="L85" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="N85" s="52" t="s">
+      <c r="M85" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="O85" s="50"/>
+      <c r="N85" s="50"/>
+      <c r="O85" s="51" t="s">
+        <v>36</v>
+      </c>
       <c r="P85" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q85" s="51" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="86" spans="8:17">
+    <row r="86" spans="7:16">
+      <c r="G86" s="50"/>
       <c r="H86" s="50"/>
       <c r="I86" s="50"/>
       <c r="J86" s="50"/>
-      <c r="K86" s="50"/>
-      <c r="L86" s="55" t="s">
+      <c r="K86" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="M86" s="53" t="s">
+      <c r="L86" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="N86" s="55" t="s">
+      <c r="M86" s="55" t="s">
         <v>125</v>
       </c>
-      <c r="O86" s="50"/>
+      <c r="N86" s="50"/>
+      <c r="O86" s="51" t="s">
+        <v>37</v>
+      </c>
       <c r="P86" s="51" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q86" s="51" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="87" spans="8:17">
+    <row r="87" spans="7:16">
+      <c r="G87" s="50"/>
       <c r="H87" s="50"/>
       <c r="I87" s="50"/>
       <c r="J87" s="50"/>
-      <c r="K87" s="50"/>
-      <c r="L87" s="57" t="s">
+      <c r="K87" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="M87" s="53" t="s">
+      <c r="L87" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="N87" s="57" t="s">
+      <c r="M87" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="O87" s="50"/>
+      <c r="N87" s="50"/>
+      <c r="O87" s="51" t="s">
+        <v>38</v>
+      </c>
       <c r="P87" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q87" s="51" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="88" spans="8:17">
+    <row r="88" spans="7:16">
+      <c r="G88" s="50"/>
       <c r="H88" s="50"/>
       <c r="I88" s="50"/>
       <c r="J88" s="50"/>
-      <c r="K88" s="50"/>
-      <c r="L88" s="57"/>
-      <c r="M88" s="53"/>
-      <c r="N88" s="57"/>
-      <c r="O88" s="50"/>
+      <c r="K88" s="57"/>
+      <c r="L88" s="53"/>
+      <c r="M88" s="57"/>
+      <c r="N88" s="50"/>
+      <c r="O88" s="51" t="s">
+        <v>40</v>
+      </c>
       <c r="P88" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q88" s="51" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="8:17">
+    <row r="89" spans="7:16">
+      <c r="G89" s="50"/>
       <c r="H89" s="50"/>
       <c r="I89" s="50"/>
       <c r="J89" s="50"/>
-      <c r="K89" s="50"/>
-      <c r="L89" s="57"/>
-      <c r="M89" s="53"/>
-      <c r="N89" s="57"/>
-      <c r="O89" s="50"/>
+      <c r="K89" s="57"/>
+      <c r="L89" s="53"/>
+      <c r="M89" s="57"/>
+      <c r="N89" s="50"/>
+      <c r="O89" s="51" t="s">
+        <v>41</v>
+      </c>
       <c r="P89" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q89" s="51" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="90" spans="8:17">
+    <row r="90" spans="7:16">
+      <c r="G90" s="50"/>
       <c r="H90" s="50"/>
       <c r="I90" s="50"/>
       <c r="J90" s="50"/>
-      <c r="K90" s="50"/>
-      <c r="L90" s="51" t="s">
+      <c r="K90" s="51" t="s">
         <v>29</v>
       </c>
+      <c r="L90" s="50"/>
       <c r="M90" s="50"/>
       <c r="N90" s="50"/>
-      <c r="O90" s="50"/>
+      <c r="O90" s="51" t="s">
+        <v>42</v>
+      </c>
       <c r="P90" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q90" s="51" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="91" spans="8:17">
+    <row r="91" spans="7:16">
+      <c r="G91" s="50"/>
       <c r="H91" s="50"/>
       <c r="I91" s="50"/>
       <c r="J91" s="50"/>
-      <c r="K91" s="50"/>
-      <c r="L91" s="52" t="s">
+      <c r="K91" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="M91" s="59" t="s">
+      <c r="L91" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="N91" s="52" t="s">
+      <c r="M91" s="52" t="s">
         <v>23</v>
       </c>
+      <c r="N91" s="50"/>
       <c r="O91" s="50"/>
       <c r="P91" s="50"/>
-      <c r="Q91" s="50"/>
-    </row>
-    <row r="92" spans="8:17">
+    </row>
+    <row r="92" spans="7:16">
+      <c r="G92" s="50"/>
       <c r="H92" s="50"/>
       <c r="I92" s="50"/>
       <c r="J92" s="50"/>
-      <c r="K92" s="50"/>
-      <c r="L92" s="65" t="s">
+      <c r="K92" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="M92" s="66" t="s">
+      <c r="L92" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="N92" s="65" t="s">
+      <c r="M92" s="55" t="s">
         <v>125</v>
       </c>
+      <c r="N92" s="50"/>
       <c r="O92" s="50"/>
       <c r="P92" s="50"/>
-      <c r="Q92" s="50"/>
-    </row>
-    <row r="93" spans="8:17">
+    </row>
+    <row r="93" spans="7:16">
+      <c r="G93" s="50"/>
       <c r="H93" s="50"/>
       <c r="I93" s="50"/>
       <c r="J93" s="50"/>
-      <c r="K93" s="50"/>
-      <c r="L93" s="57" t="s">
+      <c r="K93" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="M93" s="59" t="s">
+      <c r="L93" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="N93" s="57" t="s">
+      <c r="M93" s="57" t="s">
         <v>20</v>
       </c>
+      <c r="N93" s="50"/>
       <c r="O93" s="50"/>
       <c r="P93" s="50"/>
-      <c r="Q93" s="50"/>
-    </row>
-    <row r="94" spans="8:17">
+    </row>
+    <row r="94" spans="7:16">
+      <c r="G94" s="50"/>
       <c r="H94" s="50"/>
       <c r="I94" s="50"/>
       <c r="J94" s="50"/>
-      <c r="K94" s="50"/>
-      <c r="L94" s="52" t="s">
+      <c r="K94" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="M94" s="59" t="s">
+      <c r="L94" s="59" t="s">
         <v>127</v>
       </c>
-      <c r="N94" s="52" t="s">
+      <c r="M94" s="52" t="s">
         <v>23</v>
       </c>
+      <c r="N94" s="50"/>
       <c r="O94" s="50"/>
       <c r="P94" s="50"/>
-      <c r="Q94" s="50"/>
-    </row>
-    <row r="95" spans="8:17">
+    </row>
+    <row r="95" spans="7:16">
+      <c r="G95" s="50"/>
       <c r="H95" s="50"/>
       <c r="I95" s="50"/>
       <c r="J95" s="50"/>
-      <c r="K95" s="50"/>
-      <c r="L95" s="55" t="s">
+      <c r="K95" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="M95" s="59" t="s">
+      <c r="L95" s="59" t="s">
         <v>127</v>
       </c>
-      <c r="N95" s="55" t="s">
+      <c r="M95" s="55" t="s">
         <v>125</v>
       </c>
+      <c r="N95" s="50"/>
       <c r="O95" s="50"/>
       <c r="P95" s="50"/>
-      <c r="Q95" s="50"/>
-    </row>
-    <row r="96" spans="8:17">
+    </row>
+    <row r="96" spans="7:16">
+      <c r="G96" s="50"/>
       <c r="H96" s="50"/>
       <c r="I96" s="50"/>
       <c r="J96" s="50"/>
-      <c r="K96" s="50"/>
-      <c r="L96" s="57" t="s">
+      <c r="K96" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="M96" s="59" t="s">
+      <c r="L96" s="59" t="s">
         <v>127</v>
       </c>
-      <c r="N96" s="57" t="s">
+      <c r="M96" s="57" t="s">
         <v>20</v>
       </c>
+      <c r="N96" s="50"/>
       <c r="O96" s="50"/>
       <c r="P96" s="50"/>
-      <c r="Q96" s="50"/>
-    </row>
-    <row r="97" spans="8:17">
+    </row>
+    <row r="97" spans="7:16">
+      <c r="G97" s="50"/>
       <c r="H97" s="50"/>
       <c r="I97" s="50"/>
       <c r="J97" s="50"/>
-      <c r="K97" s="50"/>
-      <c r="L97" s="52" t="s">
+      <c r="K97" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="M97" s="59" t="s">
+      <c r="L97" s="59" t="s">
         <v>129</v>
       </c>
-      <c r="N97" s="52" t="s">
+      <c r="M97" s="52" t="s">
         <v>23</v>
       </c>
+      <c r="N97" s="50"/>
       <c r="O97" s="50"/>
       <c r="P97" s="50"/>
-      <c r="Q97" s="50"/>
-    </row>
-    <row r="98" spans="8:17">
+    </row>
+    <row r="98" spans="7:16">
+      <c r="G98" s="50"/>
       <c r="H98" s="50"/>
       <c r="I98" s="50"/>
       <c r="J98" s="50"/>
-      <c r="K98" s="50"/>
-      <c r="L98" s="55" t="s">
+      <c r="K98" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="M98" s="59" t="s">
+      <c r="L98" s="59" t="s">
         <v>129</v>
       </c>
-      <c r="N98" s="55" t="s">
+      <c r="M98" s="55" t="s">
         <v>125</v>
       </c>
+      <c r="N98" s="50"/>
       <c r="O98" s="50"/>
       <c r="P98" s="50"/>
-      <c r="Q98" s="50"/>
-    </row>
-    <row r="99" spans="8:17">
+    </row>
+    <row r="99" spans="7:16">
+      <c r="G99" s="50"/>
       <c r="H99" s="50"/>
       <c r="I99" s="50"/>
       <c r="J99" s="50"/>
-      <c r="K99" s="50"/>
-      <c r="L99" s="57" t="s">
+      <c r="K99" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="M99" s="59" t="s">
+      <c r="L99" s="59" t="s">
         <v>129</v>
       </c>
-      <c r="N99" s="57" t="s">
+      <c r="M99" s="57" t="s">
         <v>20</v>
       </c>
+      <c r="N99" s="50"/>
       <c r="O99" s="50"/>
       <c r="P99" s="50"/>
-      <c r="Q99" s="50"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4907,8 +4796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="A24" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4990,10 +4879,10 @@
       <c r="F3" t="s">
         <v>147</v>
       </c>
-      <c r="G3" s="68" t="s">
+      <c r="G3" s="64" t="s">
         <v>142</v>
       </c>
-      <c r="H3" s="68" t="s">
+      <c r="H3" s="64" t="s">
         <v>150</v>
       </c>
     </row>
@@ -5530,10 +5419,10 @@
       <c r="D24" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="68" t="s">
+      <c r="E24" s="64" t="s">
         <v>132</v>
       </c>
-      <c r="F24" s="68" t="s">
+      <c r="F24" s="64" t="s">
         <v>145</v>
       </c>
       <c r="G24" t="s">
@@ -5556,10 +5445,10 @@
       <c r="D25" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="68" t="s">
+      <c r="E25" s="64" t="s">
         <v>132</v>
       </c>
-      <c r="F25" s="68" t="s">
+      <c r="F25" s="64" t="s">
         <v>146</v>
       </c>
       <c r="G25" t="s">
@@ -5582,10 +5471,10 @@
       <c r="D26" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="68" t="s">
+      <c r="E26" s="64" t="s">
         <v>133</v>
       </c>
-      <c r="F26" s="68" t="s">
+      <c r="F26" s="64" t="s">
         <v>145</v>
       </c>
       <c r="G26" t="s">
@@ -5764,10 +5653,10 @@
       <c r="D33" t="s">
         <v>9</v>
       </c>
-      <c r="E33" s="69" t="s">
+      <c r="E33" s="65" t="s">
         <v>135</v>
       </c>
-      <c r="F33" s="69" t="s">
+      <c r="F33" s="65" t="s">
         <v>144</v>
       </c>
       <c r="G33" t="s">
@@ -5790,10 +5679,10 @@
       <c r="D34" t="s">
         <v>9</v>
       </c>
-      <c r="E34" s="70" t="s">
+      <c r="E34" s="66" t="s">
         <v>134</v>
       </c>
-      <c r="F34" s="70" t="s">
+      <c r="F34" s="66" t="s">
         <v>144</v>
       </c>
       <c r="G34" t="s">
@@ -6264,10 +6153,10 @@
       <c r="F52" t="s">
         <v>9</v>
       </c>
-      <c r="G52" s="69" t="s">
+      <c r="G52" s="65" t="s">
         <v>140</v>
       </c>
-      <c r="H52" s="69" t="s">
+      <c r="H52" s="65" t="s">
         <v>148</v>
       </c>
     </row>
@@ -6290,10 +6179,10 @@
       <c r="F53" t="s">
         <v>9</v>
       </c>
-      <c r="G53" s="69" t="s">
+      <c r="G53" s="65" t="s">
         <v>140</v>
       </c>
-      <c r="H53" s="69" t="s">
+      <c r="H53" s="65" t="s">
         <v>148</v>
       </c>
     </row>
@@ -6301,7 +6190,7 @@
       <c r="A54" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B54" s="67" t="s">
+      <c r="B54" s="63" t="s">
         <v>26</v>
       </c>
       <c r="C54" s="18" t="s">
@@ -6316,10 +6205,10 @@
       <c r="F54" t="s">
         <v>9</v>
       </c>
-      <c r="G54" s="68" t="s">
+      <c r="G54" s="64" t="s">
         <v>140</v>
       </c>
-      <c r="H54" s="68" t="s">
+      <c r="H54" s="64" t="s">
         <v>151</v>
       </c>
     </row>
@@ -6342,10 +6231,10 @@
       <c r="F55" t="s">
         <v>9</v>
       </c>
-      <c r="G55" s="68" t="s">
+      <c r="G55" s="64" t="s">
         <v>140</v>
       </c>
-      <c r="H55" s="68" t="s">
+      <c r="H55" s="64" t="s">
         <v>151</v>
       </c>
     </row>
@@ -6602,10 +6491,10 @@
       <c r="F65" t="s">
         <v>147</v>
       </c>
-      <c r="G65" s="68" t="s">
+      <c r="G65" s="64" t="s">
         <v>146</v>
       </c>
-      <c r="H65" s="68" t="s">
+      <c r="H65" s="64" t="s">
         <v>150</v>
       </c>
     </row>

</xml_diff>